<commit_message>
Remove pywin32 from requirements to deploy
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Said\Desktop\gazi\Yapay Zeka Öğrenme Modelleri\Proje_Odevi\project_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81C618DA-2CB2-44A6-AC91-8A15E88422BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56914EB2-45AC-4AE5-8A9C-F456FDDEB3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7815" yWindow="0" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Model</t>
   </si>
@@ -168,11 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,558 +511,720 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.53</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.69</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0.76</v>
       </c>
-      <c r="E2">
-        <v>0.79</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="F2" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>0.49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0.52</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.71</v>
       </c>
-      <c r="D3">
-        <v>0.79</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="E3" s="2">
         <v>0.86</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.63</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.44</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0.54</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.72</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.83</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.87</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>0.65</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>0.46</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.69</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.66</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.75</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>0.51</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.68</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.63</v>
       </c>
-      <c r="E6">
-        <v>0.79</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="F6" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>0.47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0.59</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.72</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.69</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.8</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.61</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.72</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.68</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.81</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>0.61</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>0.54</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.51</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.68</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.63</v>
       </c>
-      <c r="E9">
-        <v>0.79</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="F9" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>0.47</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0.59</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>0.72</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.69</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0.8</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>0.61</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>0.62</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>0.72</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.8</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>0.76</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>0.6</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0.65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>0.64</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>0.72</v>
       </c>
-      <c r="D12">
-        <v>0.79</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="E12" s="2">
         <v>0.73</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>0.59</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>0.72</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>0.65</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>0.75</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>0.84</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>0.81</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>0.65</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>0.65</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>0.65</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>0.75</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0.83</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>0.8</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>0.64</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>0.67</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>0.64</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>0.72</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0.8</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>0.73</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>0.59</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>0.72</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>0.65</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>0.75</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>0.84</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>0.81</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>0.65</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>0.65</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>0.67</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>0.76</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>0.84</v>
       </c>
-      <c r="E17">
-        <v>0.79</v>
-      </c>
-      <c r="F17">
+      <c r="E17" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="F17" s="2">
         <v>0.65</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>0.7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>0.64</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>0.72</v>
       </c>
-      <c r="D18">
-        <v>0.79</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="E18" s="2">
         <v>0.73</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>0.59</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>0.7</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>0.67</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>0.75</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>0.84</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>0.78</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>0.63</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>0.7</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20">
-        <v>0.79</v>
-      </c>
-      <c r="C20">
-        <v>0.79</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="D20" s="2">
         <v>0.86</v>
       </c>
-      <c r="E20">
-        <v>0.79</v>
-      </c>
-      <c r="F20">
-        <v>0.79</v>
-      </c>
-      <c r="G20">
+      <c r="E20" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="F20" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="G20" s="2">
         <v>0.79</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>0.78</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="2">
         <v>0.78</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>0.86</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>0.78</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>0.78</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>0.77</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="2">
         <v>0.74</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="2">
         <v>0.74</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>0.81</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>0.73</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>0.74</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B23">
-        <v>0.77</v>
-      </c>
-      <c r="C23">
-        <v>0.77</v>
-      </c>
-      <c r="D23">
+      <c r="B23" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="D23" s="2">
         <v>0.86</v>
       </c>
-      <c r="E23">
-        <v>0.77</v>
-      </c>
-      <c r="F23">
-        <v>0.77</v>
-      </c>
-      <c r="G23">
+      <c r="E23" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="G23" s="2">
         <v>0.77</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="2">
         <v>0.45</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>0.75</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>0.81</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>0.65</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>0.35</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B25">
-        <v>0.77</v>
-      </c>
-      <c r="C25">
-        <v>0.77</v>
-      </c>
-      <c r="D25">
+      <c r="B25" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="D25" s="2">
         <v>0.86</v>
       </c>
-      <c r="E25">
-        <v>0.77</v>
-      </c>
-      <c r="F25">
-        <v>0.77</v>
-      </c>
-      <c r="G25">
+      <c r="E25" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="F25" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="F29" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.81</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="G32" s="2">
         <v>0.77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>